<commit_message>
validacion formato de entrada
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="209">
   <si>
     <t>PUNTO_VENTA</t>
   </si>
@@ -815,7 +815,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -860,15 +860,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1965,7 +1956,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2015,7 +2006,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2065,7 +2056,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -2115,7 +2106,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2165,7 +2156,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -6632,10 +6623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6648,17 +6639,14 @@
     <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -6683,32 +6671,23 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="str">
         <f>+VLOOKUP(B2,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA ARKADIA</v>
@@ -6734,32 +6713,23 @@
       <c r="H2" s="8">
         <v>1127</v>
       </c>
-      <c r="I2" s="4">
-        <v>2.966199</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="15">
-        <v>1</v>
-      </c>
-      <c r="L2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M2" s="8">
+      <c r="J2" s="8">
         <v>1319</v>
       </c>
-      <c r="N2" s="5">
+      <c r="K2" s="5">
         <v>300733.92600000027</v>
       </c>
-      <c r="O2" s="11">
+      <c r="L2" s="11">
         <v>5.3814216625604525E-2</v>
       </c>
-      <c r="P2" s="4">
+      <c r="M2" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="str">
         <f>+VLOOKUP(B3,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA  VIVA ENVIGADO</v>
@@ -6785,32 +6755,23 @@
       <c r="H3" s="8">
         <v>895</v>
       </c>
-      <c r="I3" s="4">
-        <v>2.5366140000000001</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="15">
-        <v>2</v>
-      </c>
-      <c r="L3" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M3" s="8">
+      <c r="J3" s="8">
         <v>1033</v>
       </c>
-      <c r="N3" s="5">
+      <c r="K3" s="5">
         <v>331133.66800000024</v>
       </c>
-      <c r="O3" s="11">
+      <c r="L3" s="11">
         <v>3.0010734092671E-2</v>
       </c>
-      <c r="P3" s="4">
+      <c r="M3" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="str">
         <f>+VLOOKUP(B4,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>VENTURA PLAZA CUCUTA</v>
@@ -6836,32 +6797,23 @@
       <c r="H4" s="8">
         <v>798</v>
       </c>
-      <c r="I4" s="4">
-        <v>2.2505289999999998</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="15">
-        <v>3</v>
-      </c>
-      <c r="L4" s="15" t="s">
+      <c r="I4" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M4" s="8">
+      <c r="J4" s="8">
         <v>933</v>
       </c>
-      <c r="N4" s="5">
+      <c r="K4" s="5">
         <v>283012.1210000001</v>
       </c>
-      <c r="O4" s="11">
+      <c r="L4" s="11">
         <v>2.3386426437220588E-2</v>
       </c>
-      <c r="P4" s="4">
+      <c r="M4" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="str">
         <f>+VLOOKUP(B5,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA SAN DIEGO</v>
@@ -6887,32 +6839,23 @@
       <c r="H5" s="8">
         <v>887</v>
       </c>
-      <c r="I5" s="4">
-        <v>2.2084549999999998</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="15">
-        <v>4</v>
-      </c>
-      <c r="L5" s="15" t="s">
+      <c r="I5" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M5" s="8">
+      <c r="J5" s="8">
         <v>1055</v>
       </c>
-      <c r="N5" s="5">
+      <c r="K5" s="5">
         <v>297045.61800000025</v>
       </c>
-      <c r="O5" s="11">
+      <c r="L5" s="11">
         <v>3.7485556839392052E-2</v>
       </c>
-      <c r="P5" s="4">
+      <c r="M5" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="str">
         <f>+VLOOKUP(B6,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA MAYORCA</v>
@@ -6938,32 +6881,23 @@
       <c r="H6" s="8">
         <v>822</v>
       </c>
-      <c r="I6" s="4">
-        <v>2.191551</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="15">
-        <v>5</v>
-      </c>
-      <c r="L6" s="15" t="s">
+      <c r="I6" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M6" s="8">
+      <c r="J6" s="8">
         <v>959</v>
       </c>
-      <c r="N6" s="5">
+      <c r="K6" s="5">
         <v>285718.74100000027</v>
       </c>
-      <c r="O6" s="11">
+      <c r="L6" s="11">
         <v>3.4711790788163964E-2</v>
       </c>
-      <c r="P6" s="4">
+      <c r="M6" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="str">
         <f>+VLOOKUP(B7,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA  PLAZA FABRICATO</v>
@@ -6989,32 +6923,23 @@
       <c r="H7" s="8">
         <v>673</v>
       </c>
-      <c r="I7" s="4">
-        <v>2.0937990000000002</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="15">
-        <v>6</v>
-      </c>
-      <c r="L7" s="15" t="s">
+      <c r="I7" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M7" s="8">
+      <c r="J7" s="8">
         <v>806</v>
       </c>
-      <c r="N7" s="5">
+      <c r="K7" s="5">
         <v>323481.52600000007</v>
       </c>
-      <c r="O7" s="11">
+      <c r="L7" s="11">
         <v>3.3935712256626532E-2</v>
       </c>
-      <c r="P7" s="4">
+      <c r="M7" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="str">
         <f>+VLOOKUP(B8,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA JARDIN PLAZA</v>
@@ -7040,32 +6965,23 @@
       <c r="H8" s="8">
         <v>740</v>
       </c>
-      <c r="I8" s="4">
-        <v>2.0686290000000001</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="15">
-        <v>7</v>
-      </c>
-      <c r="L8" s="15" t="s">
+      <c r="I8" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M8" s="8">
+      <c r="J8" s="8">
         <v>895</v>
       </c>
-      <c r="N8" s="5">
+      <c r="K8" s="5">
         <v>308450.8000000001</v>
       </c>
-      <c r="O8" s="11">
+      <c r="L8" s="11">
         <v>2.5538438528268023E-2</v>
       </c>
-      <c r="P8" s="4">
+      <c r="M8" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="str">
         <f>+VLOOKUP(B9,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA CHIPICHAPE 2</v>
@@ -7091,32 +7007,23 @@
       <c r="H9" s="8">
         <v>830</v>
       </c>
-      <c r="I9" s="4">
-        <v>2.044133</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="15">
-        <v>8</v>
-      </c>
-      <c r="L9" s="15" t="s">
+      <c r="I9" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M9" s="8">
+      <c r="J9" s="8">
         <v>971</v>
       </c>
-      <c r="N9" s="5">
+      <c r="K9" s="5">
         <v>285685.31200000009</v>
       </c>
-      <c r="O9" s="11">
+      <c r="L9" s="11">
         <v>2.7155718572857618E-2</v>
       </c>
-      <c r="P9" s="4">
+      <c r="M9" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="str">
         <f>+VLOOKUP(B10,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA LOS MOLINOS</v>
@@ -7142,32 +7049,23 @@
       <c r="H10" s="8">
         <v>667</v>
       </c>
-      <c r="I10" s="4">
-        <v>1.918102</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="15">
-        <v>9</v>
-      </c>
-      <c r="L10" s="15" t="s">
+      <c r="I10" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M10" s="8">
+      <c r="J10" s="8">
         <v>809</v>
       </c>
-      <c r="N10" s="5">
+      <c r="K10" s="5">
         <v>320724.30500000017</v>
       </c>
-      <c r="O10" s="11">
+      <c r="L10" s="11">
         <v>2.4037764423464208E-2</v>
       </c>
-      <c r="P10" s="4">
+      <c r="M10" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="str">
         <f>+VLOOKUP(B11,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA EL TESORO</v>
@@ -7193,32 +7091,23 @@
       <c r="H11" s="8">
         <v>667</v>
       </c>
-      <c r="I11" s="4">
-        <v>1.8153509999999999</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="15">
+      <c r="I11" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="J11" s="8">
+        <v>828</v>
+      </c>
+      <c r="K11" s="5">
+        <v>308454.86000000016</v>
+      </c>
+      <c r="L11" s="11">
+        <v>2.5012433435631195E-2</v>
+      </c>
+      <c r="M11" s="4">
         <v>10</v>
       </c>
-      <c r="L11" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="M11" s="8">
-        <v>828</v>
-      </c>
-      <c r="N11" s="5">
-        <v>308454.86000000016</v>
-      </c>
-      <c r="O11" s="11">
-        <v>2.5012433435631195E-2</v>
-      </c>
-      <c r="P11" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="str">
         <f>+VLOOKUP(B12,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>GRAN PLAZA FLORENCIA</v>
@@ -7244,32 +7133,23 @@
       <c r="H12" s="8">
         <v>641</v>
       </c>
-      <c r="I12" s="4">
-        <v>1.514386</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="15">
-        <v>11</v>
-      </c>
-      <c r="L12" s="15" t="s">
+      <c r="I12" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M12" s="8">
+      <c r="J12" s="8">
         <v>765</v>
       </c>
-      <c r="N12" s="5">
+      <c r="K12" s="5">
         <v>280240.96100000001</v>
       </c>
-      <c r="O12" s="11">
+      <c r="L12" s="11">
         <v>3.0561017929438983E-2</v>
       </c>
-      <c r="P12" s="4">
+      <c r="M12" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="str">
         <f>+VLOOKUP(B13,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>UNICENTRO ARMENIA</v>
@@ -7295,32 +7175,23 @@
       <c r="H13" s="8">
         <v>582</v>
       </c>
-      <c r="I13" s="4">
-        <v>1.4863770000000001</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="15">
-        <v>12</v>
-      </c>
-      <c r="L13" s="15" t="s">
+      <c r="I13" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M13" s="8">
+      <c r="J13" s="8">
         <v>719</v>
       </c>
-      <c r="N13" s="5">
+      <c r="K13" s="5">
         <v>309636.02400000027</v>
       </c>
-      <c r="O13" s="11">
+      <c r="L13" s="11">
         <v>2.9322800789940755E-2</v>
       </c>
-      <c r="P13" s="4">
+      <c r="M13" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="str">
         <f>+VLOOKUP(B14,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA CENTRO MAYOR</v>
@@ -7346,32 +7217,23 @@
       <c r="H14" s="8">
         <v>538</v>
       </c>
-      <c r="I14" s="4">
-        <v>1.286772</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="15">
-        <v>13</v>
-      </c>
-      <c r="L14" s="15" t="s">
+      <c r="I14" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M14" s="8">
+      <c r="J14" s="8">
         <v>671</v>
       </c>
-      <c r="N14" s="5">
+      <c r="K14" s="5">
         <v>308435.34700000013</v>
       </c>
-      <c r="O14" s="11">
+      <c r="L14" s="11">
         <v>2.4321621667429367E-2</v>
       </c>
-      <c r="P14" s="4">
+      <c r="M14" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="str">
         <f>+VLOOKUP(B15,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA UNICENTRO CALI</v>
@@ -7397,32 +7259,23 @@
       <c r="H15" s="8">
         <v>632</v>
       </c>
-      <c r="I15" s="4">
-        <v>1.260877</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="15">
-        <v>14</v>
-      </c>
-      <c r="L15" s="15" t="s">
+      <c r="I15" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M15" s="8">
+      <c r="J15" s="8">
         <v>774</v>
       </c>
-      <c r="N15" s="5">
+      <c r="K15" s="5">
         <v>245396.05800000014</v>
       </c>
-      <c r="O15" s="11">
+      <c r="L15" s="11">
         <v>2.3717092004497339E-2</v>
       </c>
-      <c r="P15" s="4">
+      <c r="M15" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="str">
         <f>+VLOOKUP(B16,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA SANTAFÉ MEDELLIN</v>
@@ -7448,32 +7301,23 @@
       <c r="H16" s="8">
         <v>643</v>
       </c>
-      <c r="I16" s="4">
-        <v>1.2379020000000001</v>
-      </c>
-      <c r="J16" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" s="15">
-        <v>15</v>
-      </c>
-      <c r="L16" s="15" t="s">
+      <c r="I16" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M16" s="8">
+      <c r="J16" s="8">
         <v>786</v>
       </c>
-      <c r="N16" s="5">
+      <c r="K16" s="5">
         <v>285654.16100000002</v>
       </c>
-      <c r="O16" s="11">
+      <c r="L16" s="11">
         <v>2.7473052910558887E-2</v>
       </c>
-      <c r="P16" s="4">
+      <c r="M16" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="str">
         <f>+VLOOKUP(B17,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>FUNDADORES MANIZALES</v>
@@ -7499,32 +7343,23 @@
       <c r="H17" s="8">
         <v>560</v>
       </c>
-      <c r="I17" s="4">
-        <v>1.184563</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="15">
-        <v>16</v>
-      </c>
-      <c r="L17" s="15" t="s">
+      <c r="I17" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M17" s="8">
+      <c r="J17" s="8">
         <v>757</v>
       </c>
-      <c r="N17" s="5">
+      <c r="K17" s="5">
         <v>323426.56700000016</v>
       </c>
-      <c r="O17" s="11">
+      <c r="L17" s="11">
         <v>3.6664247625658661E-2</v>
       </c>
-      <c r="P17" s="4">
+      <c r="M17" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="str">
         <f>+VLOOKUP(B18,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA VIVA LA CEJA</v>
@@ -7550,32 +7385,23 @@
       <c r="H18" s="8">
         <v>561</v>
       </c>
-      <c r="I18" s="4">
-        <v>1.1068009999999999</v>
-      </c>
-      <c r="J18" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="15">
-        <v>17</v>
-      </c>
-      <c r="L18" s="15" t="s">
+      <c r="I18" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M18" s="8">
+      <c r="J18" s="8">
         <v>704</v>
       </c>
-      <c r="N18" s="5">
+      <c r="K18" s="5">
         <v>237570.79300000009</v>
       </c>
-      <c r="O18" s="11">
+      <c r="L18" s="11">
         <v>5.6185690356544631E-2</v>
       </c>
-      <c r="P18" s="4">
+      <c r="M18" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="str">
         <f>+VLOOKUP(B19,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA PLAZA CENTRAL</v>
@@ -7601,32 +7427,23 @@
       <c r="H19" s="8">
         <v>502</v>
       </c>
-      <c r="I19" s="4">
-        <v>1.072308</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" s="15">
-        <v>18</v>
-      </c>
-      <c r="L19" s="15" t="s">
+      <c r="I19" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M19" s="8">
+      <c r="J19" s="8">
         <v>636</v>
       </c>
-      <c r="N19" s="5">
+      <c r="K19" s="5">
         <v>323413.81600000017</v>
       </c>
-      <c r="O19" s="11">
+      <c r="L19" s="11">
         <v>2.8360488798370671E-2</v>
       </c>
-      <c r="P19" s="4">
+      <c r="M19" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="str">
         <f>+VLOOKUP(B20,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>VIVA WAJIRA</v>
@@ -7652,32 +7469,23 @@
       <c r="H20" s="8">
         <v>518</v>
       </c>
-      <c r="I20" s="4">
-        <v>1.0549580000000001</v>
-      </c>
-      <c r="J20" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K20" s="15">
-        <v>19</v>
-      </c>
-      <c r="L20" s="15" t="s">
+      <c r="I20" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M20" s="8">
+      <c r="J20" s="8">
         <v>662</v>
       </c>
-      <c r="N20" s="5">
+      <c r="K20" s="5">
         <v>293008.33400000021</v>
       </c>
-      <c r="O20" s="11">
+      <c r="L20" s="11">
         <v>2.3569682151589243E-2</v>
       </c>
-      <c r="P20" s="4">
+      <c r="M20" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="str">
         <f>+VLOOKUP(B21,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA TITÁN PLAZA</v>
@@ -7703,32 +7511,23 @@
       <c r="H21" s="8">
         <v>499</v>
       </c>
-      <c r="I21" s="4">
-        <v>0.92637899999999995</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K21" s="15">
-        <v>20</v>
-      </c>
-      <c r="L21" s="15" t="s">
+      <c r="I21" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M21" s="8">
+      <c r="J21" s="8">
         <v>650</v>
       </c>
-      <c r="N21" s="5">
+      <c r="K21" s="5">
         <v>323398.58799999999</v>
       </c>
-      <c r="O21" s="11">
+      <c r="L21" s="11">
         <v>3.0834053586862576E-2</v>
       </c>
-      <c r="P21" s="4">
+      <c r="M21" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="str">
         <f>+VLOOKUP(B22,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>CARIBE PLAZA CARTAGENA</v>
@@ -7754,32 +7553,23 @@
       <c r="H22" s="8">
         <v>488</v>
       </c>
-      <c r="I22" s="4">
-        <v>0.91451899999999997</v>
-      </c>
-      <c r="J22" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K22" s="15">
-        <v>21</v>
-      </c>
-      <c r="L22" s="15" t="s">
+      <c r="I22" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M22" s="8">
+      <c r="J22" s="8">
         <v>616</v>
       </c>
-      <c r="N22" s="5">
+      <c r="K22" s="5">
         <v>300961.60900000005</v>
       </c>
-      <c r="O22" s="11">
+      <c r="L22" s="11">
         <v>1.7207101254480286E-2</v>
       </c>
-      <c r="P22" s="4">
+      <c r="M22" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="str">
         <f>+VLOOKUP(B23,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA CENTRO ANDINO</v>
@@ -7805,32 +7595,23 @@
       <c r="H23" s="8">
         <v>560</v>
       </c>
-      <c r="I23" s="4">
-        <v>0.83009999999999995</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K23" s="15">
-        <v>22</v>
-      </c>
-      <c r="L23" s="15" t="s">
+      <c r="I23" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M23" s="8">
+      <c r="J23" s="8">
         <v>744</v>
       </c>
-      <c r="N23" s="5">
+      <c r="K23" s="5">
         <v>262968.26500000007</v>
       </c>
-      <c r="O23" s="11">
+      <c r="L23" s="11">
         <v>2.3791250959324637E-2</v>
       </c>
-      <c r="P23" s="4">
+      <c r="M23" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="str">
         <f>+VLOOKUP(B24,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA SAN NICOLÁS</v>
@@ -7856,32 +7637,23 @@
       <c r="H24" s="8">
         <v>510</v>
       </c>
-      <c r="I24" s="4">
-        <v>0.81694699999999998</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K24" s="15">
-        <v>23</v>
-      </c>
-      <c r="L24" s="15" t="s">
+      <c r="I24" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M24" s="8">
+      <c r="J24" s="8">
         <v>681</v>
       </c>
-      <c r="N24" s="5">
+      <c r="K24" s="5">
         <v>266643.96500000008</v>
       </c>
-      <c r="O24" s="11">
+      <c r="L24" s="11">
         <v>2.6659496004917026E-2</v>
       </c>
-      <c r="P24" s="4">
+      <c r="M24" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="str">
         <f>+VLOOKUP(B25,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>OFFCORSS ARAUCA</v>
@@ -7907,32 +7679,23 @@
       <c r="H25" s="8">
         <v>442</v>
       </c>
-      <c r="I25" s="4">
-        <v>0.81650900000000004</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K25" s="15">
-        <v>24</v>
-      </c>
-      <c r="L25" s="15" t="s">
+      <c r="I25" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M25" s="8">
+      <c r="J25" s="8">
         <v>567</v>
       </c>
-      <c r="N25" s="5">
+      <c r="K25" s="5">
         <v>278730.72100000002</v>
       </c>
-      <c r="O25" s="11">
+      <c r="L25" s="11">
         <v>3.2365452191603479E-2</v>
       </c>
-      <c r="P25" s="4">
+      <c r="M25" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="str">
         <f>+VLOOKUP(B26,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA VIVA VILLAVICENCIO</v>
@@ -7958,32 +7721,23 @@
       <c r="H26" s="8">
         <v>555</v>
       </c>
-      <c r="I26" s="4">
-        <v>0.79765799999999998</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K26" s="15">
-        <v>25</v>
-      </c>
-      <c r="L26" s="15" t="s">
+      <c r="I26" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M26" s="8">
+      <c r="J26" s="8">
         <v>681</v>
       </c>
-      <c r="N26" s="5">
+      <c r="K26" s="5">
         <v>264124.36599999998</v>
       </c>
-      <c r="O26" s="11">
+      <c r="L26" s="11">
         <v>1.9972315602135655E-2</v>
       </c>
-      <c r="P26" s="4">
+      <c r="M26" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="str">
         <f>+VLOOKUP(B27,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA UNICENTRO GIRARDOT</v>
@@ -8009,32 +7763,23 @@
       <c r="H27" s="8">
         <v>482</v>
       </c>
-      <c r="I27" s="4">
-        <v>0.78750799999999999</v>
-      </c>
-      <c r="J27" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K27" s="15">
-        <v>26</v>
-      </c>
-      <c r="L27" s="15" t="s">
+      <c r="I27" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M27" s="8">
+      <c r="J27" s="8">
         <v>613</v>
       </c>
-      <c r="N27" s="5">
+      <c r="K27" s="5">
         <v>285686.35500000004</v>
       </c>
-      <c r="O27" s="11">
+      <c r="L27" s="11">
         <v>3.1519575315195753E-2</v>
       </c>
-      <c r="P27" s="4">
+      <c r="M27" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="str">
         <f>+VLOOKUP(B28,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>LA ESTACION IBAGUE</v>
@@ -8060,32 +7805,23 @@
       <c r="H28" s="8">
         <v>549</v>
       </c>
-      <c r="I28" s="4">
-        <v>0.73089899999999997</v>
-      </c>
-      <c r="J28" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K28" s="15">
-        <v>27</v>
-      </c>
-      <c r="L28" s="15" t="s">
+      <c r="I28" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M28" s="8">
+      <c r="J28" s="8">
         <v>694</v>
       </c>
-      <c r="N28" s="5">
+      <c r="K28" s="5">
         <v>275195.89200000011</v>
       </c>
-      <c r="O28" s="11">
+      <c r="L28" s="11">
         <v>2.9637115296279284E-2</v>
       </c>
-      <c r="P28" s="4">
+      <c r="M28" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="str">
         <f>+VLOOKUP(B29,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA PALMETTO</v>
@@ -8111,32 +7847,23 @@
       <c r="H29" s="8">
         <v>479</v>
       </c>
-      <c r="I29" s="4">
-        <v>0.71010399999999996</v>
-      </c>
-      <c r="J29" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K29" s="15">
-        <v>28</v>
-      </c>
-      <c r="L29" s="15" t="s">
+      <c r="I29" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M29" s="8">
+      <c r="J29" s="8">
         <v>646</v>
       </c>
-      <c r="N29" s="5">
+      <c r="K29" s="5">
         <v>278907.32700000011</v>
       </c>
-      <c r="O29" s="11">
+      <c r="L29" s="11">
         <v>2.4937544610992148E-2</v>
       </c>
-      <c r="P29" s="4">
+      <c r="M29" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="str">
         <f>+VLOOKUP(B30,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA PLAZA IMPERIAL BOGOTA</v>
@@ -8162,32 +7889,23 @@
       <c r="H30" s="8">
         <v>468</v>
       </c>
-      <c r="I30" s="4">
-        <v>0.69062599999999996</v>
-      </c>
-      <c r="J30" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K30" s="15">
-        <v>29</v>
-      </c>
-      <c r="L30" s="15" t="s">
+      <c r="I30" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M30" s="8">
+      <c r="J30" s="8">
         <v>594</v>
       </c>
-      <c r="N30" s="5">
+      <c r="K30" s="5">
         <v>280212.9470000001</v>
       </c>
-      <c r="O30" s="11">
+      <c r="L30" s="11">
         <v>3.3338325595327241E-2</v>
       </c>
-      <c r="P30" s="4">
+      <c r="M30" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="str">
         <f>+VLOOKUP(B31,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA GRAN ESTACION</v>
@@ -8213,32 +7931,23 @@
       <c r="H31" s="8">
         <v>450</v>
       </c>
-      <c r="I31" s="4">
-        <v>0.66369100000000003</v>
-      </c>
-      <c r="J31" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K31" s="15">
-        <v>30</v>
-      </c>
-      <c r="L31" s="15" t="s">
+      <c r="I31" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M31" s="8">
+      <c r="J31" s="8">
         <v>580</v>
       </c>
-      <c r="N31" s="5">
+      <c r="K31" s="5">
         <v>262993.70100000006</v>
       </c>
-      <c r="O31" s="11">
+      <c r="L31" s="11">
         <v>2.4899581932945322E-2</v>
       </c>
-      <c r="P31" s="4">
+      <c r="M31" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="str">
         <f>+VLOOKUP(B32,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>PITALITO HUILA</v>
@@ -8264,32 +7973,23 @@
       <c r="H32" s="8">
         <v>473</v>
       </c>
-      <c r="I32" s="4">
-        <v>0.66221699999999994</v>
-      </c>
-      <c r="J32" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K32" s="15">
-        <v>31</v>
-      </c>
-      <c r="L32" s="15" t="s">
+      <c r="I32" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M32" s="8">
+      <c r="J32" s="8">
         <v>592</v>
       </c>
-      <c r="N32" s="5">
+      <c r="K32" s="5">
         <v>227107.43000000008</v>
       </c>
-      <c r="O32" s="11">
+      <c r="L32" s="11">
         <v>2.4426774740644478E-2</v>
       </c>
-      <c r="P32" s="4">
+      <c r="M32" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="str">
         <f>+VLOOKUP(B33,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA GUACARI</v>
@@ -8315,32 +8015,23 @@
       <c r="H33" s="8">
         <v>478</v>
       </c>
-      <c r="I33" s="4">
-        <v>0.63166800000000001</v>
-      </c>
-      <c r="J33" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K33" s="15">
-        <v>32</v>
-      </c>
-      <c r="L33" s="15" t="s">
+      <c r="I33" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M33" s="8">
+      <c r="J33" s="8">
         <v>599</v>
       </c>
-      <c r="N33" s="5">
+      <c r="K33" s="5">
         <v>331048.11700000026</v>
       </c>
-      <c r="O33" s="11">
+      <c r="L33" s="11">
         <v>2.7464917552982988E-2</v>
       </c>
-      <c r="P33" s="4">
+      <c r="M33" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="str">
         <f>+VLOOKUP(B34,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>GUATAPURI VALLEDUPAR</v>
@@ -8366,32 +8057,23 @@
       <c r="H34" s="8">
         <v>469</v>
       </c>
-      <c r="I34" s="4">
-        <v>0.62398299999999995</v>
-      </c>
-      <c r="J34" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K34" s="15">
-        <v>33</v>
-      </c>
-      <c r="L34" s="15" t="s">
+      <c r="I34" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M34" s="8">
+      <c r="J34" s="8">
         <v>613</v>
       </c>
-      <c r="N34" s="5">
+      <c r="K34" s="5">
         <v>275241.80400000012</v>
       </c>
-      <c r="O34" s="11">
+      <c r="L34" s="11">
         <v>2.3862622658340767E-2</v>
       </c>
-      <c r="P34" s="4">
+      <c r="M34" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="15" t="str">
         <f>+VLOOKUP(B35,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA LLANOGRANDE PLAZA</v>
@@ -8417,32 +8099,23 @@
       <c r="H35" s="8">
         <v>421</v>
       </c>
-      <c r="I35" s="4">
-        <v>0.59758800000000001</v>
-      </c>
-      <c r="J35" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K35" s="15">
-        <v>34</v>
-      </c>
-      <c r="L35" s="15" t="s">
+      <c r="I35" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M35" s="8">
+      <c r="J35" s="8">
         <v>547</v>
       </c>
-      <c r="N35" s="5">
+      <c r="K35" s="5">
         <v>286878.03900000016</v>
       </c>
-      <c r="O35" s="11">
+      <c r="L35" s="11">
         <v>2.9915387924853005E-2</v>
       </c>
-      <c r="P35" s="4">
+      <c r="M35" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="str">
         <f>+VLOOKUP(B36,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA NUESTRO CARTAGO</v>
@@ -8468,32 +8141,23 @@
       <c r="H36" s="8">
         <v>475</v>
       </c>
-      <c r="I36" s="4">
-        <v>0.55964999999999998</v>
-      </c>
-      <c r="J36" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K36" s="15">
-        <v>35</v>
-      </c>
-      <c r="L36" s="15" t="s">
+      <c r="I36" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M36" s="8">
+      <c r="J36" s="8">
         <v>618</v>
       </c>
-      <c r="N36" s="5">
+      <c r="K36" s="5">
         <v>204555.56200000001</v>
       </c>
-      <c r="O36" s="11">
+      <c r="L36" s="11">
         <v>2.919116764670587E-2</v>
       </c>
-      <c r="P36" s="4">
+      <c r="M36" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="str">
         <f>+VLOOKUP(B37,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA LA FELICIDAD</v>
@@ -8519,32 +8183,23 @@
       <c r="H37" s="8">
         <v>467</v>
       </c>
-      <c r="I37" s="4">
-        <v>0.52659800000000001</v>
-      </c>
-      <c r="J37" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K37" s="15">
-        <v>36</v>
-      </c>
-      <c r="L37" s="15" t="s">
+      <c r="I37" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M37" s="8">
+      <c r="J37" s="8">
         <v>610</v>
       </c>
-      <c r="N37" s="5">
+      <c r="K37" s="5">
         <v>297004.35700000025</v>
       </c>
-      <c r="O37" s="11">
+      <c r="L37" s="11">
         <v>2.4428243870891882E-2</v>
       </c>
-      <c r="P37" s="4">
+      <c r="M37" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="str">
         <f>+VLOOKUP(B38,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>SAN PEDRO PLAZA NEIVA</v>
@@ -8570,32 +8225,23 @@
       <c r="H38" s="8">
         <v>588</v>
       </c>
-      <c r="I38" s="4">
-        <v>0.48395700000000003</v>
-      </c>
-      <c r="J38" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K38" s="15">
-        <v>37</v>
-      </c>
-      <c r="L38" s="15" t="s">
+      <c r="I38" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M38" s="8">
+      <c r="J38" s="8">
         <v>726</v>
       </c>
-      <c r="N38" s="5">
+      <c r="K38" s="5">
         <v>215654.30599999998</v>
       </c>
-      <c r="O38" s="11">
+      <c r="L38" s="11">
         <v>3.4323451890899401E-2</v>
       </c>
-      <c r="P38" s="4">
+      <c r="M38" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="str">
         <f>+VLOOKUP(B39,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA GRAN PLAZA SOACHA</v>
@@ -8621,32 +8267,23 @@
       <c r="H39" s="8">
         <v>405</v>
       </c>
-      <c r="I39" s="4">
-        <v>0.45668399999999998</v>
-      </c>
-      <c r="J39" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K39" s="15">
-        <v>38</v>
-      </c>
-      <c r="L39" s="15" t="s">
+      <c r="I39" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M39" s="8">
+      <c r="J39" s="8">
         <v>538</v>
       </c>
-      <c r="N39" s="5">
+      <c r="K39" s="5">
         <v>294306.63600000012</v>
       </c>
-      <c r="O39" s="11">
+      <c r="L39" s="11">
         <v>2.8185658994888764E-2</v>
       </c>
-      <c r="P39" s="4">
+      <c r="M39" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="str">
         <f>+VLOOKUP(B40,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>PARQUE CARACOLI</v>
@@ -8672,32 +8309,23 @@
       <c r="H40" s="8">
         <v>438</v>
       </c>
-      <c r="I40" s="4">
-        <v>0.40729799999999999</v>
-      </c>
-      <c r="J40" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K40" s="15">
-        <v>39</v>
-      </c>
-      <c r="L40" s="15" t="s">
+      <c r="I40" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M40" s="8">
+      <c r="J40" s="8">
         <v>569</v>
       </c>
-      <c r="N40" s="5">
+      <c r="K40" s="5">
         <v>260228.11400000012</v>
       </c>
-      <c r="O40" s="11">
+      <c r="L40" s="11">
         <v>2.0783520323707928E-2</v>
       </c>
-      <c r="P40" s="4">
+      <c r="M40" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="str">
         <f>+VLOOKUP(B41,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA COSMOCENTRO CALI</v>
@@ -8723,32 +8351,23 @@
       <c r="H41" s="8">
         <v>411</v>
       </c>
-      <c r="I41" s="4">
-        <v>0.31916499999999998</v>
-      </c>
-      <c r="J41" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K41" s="15">
-        <v>40</v>
-      </c>
-      <c r="L41" s="15" t="s">
+      <c r="I41" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M41" s="8">
+      <c r="J41" s="8">
         <v>556</v>
       </c>
-      <c r="N41" s="5">
+      <c r="K41" s="5">
         <v>274320.14700000011</v>
       </c>
-      <c r="O41" s="11">
+      <c r="L41" s="11">
         <v>2.595748294505619E-2</v>
       </c>
-      <c r="P41" s="4">
+      <c r="M41" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="str">
         <f>+VLOOKUP(B42,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA FUSAGASUGA</v>
@@ -8774,32 +8393,23 @@
       <c r="H42" s="8">
         <v>395</v>
       </c>
-      <c r="I42" s="4">
-        <v>0.249556</v>
-      </c>
-      <c r="J42" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K42" s="15">
-        <v>41</v>
-      </c>
-      <c r="L42" s="15" t="s">
+      <c r="I42" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M42" s="8">
+      <c r="J42" s="8">
         <v>522</v>
       </c>
-      <c r="N42" s="5">
+      <c r="K42" s="5">
         <v>280195.55200000014</v>
       </c>
-      <c r="O42" s="11">
+      <c r="L42" s="11">
         <v>4.1048268485091591E-2</v>
       </c>
-      <c r="P42" s="4">
+      <c r="M42" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="15" t="str">
         <f>+VLOOKUP(B43,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>BUENAVISTA MONTERIA</v>
@@ -8825,32 +8435,23 @@
       <c r="H43" s="8">
         <v>460</v>
       </c>
-      <c r="I43" s="4">
-        <v>0.184859</v>
-      </c>
-      <c r="J43" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K43" s="15">
-        <v>42</v>
-      </c>
-      <c r="L43" s="15" t="s">
+      <c r="I43" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M43" s="8">
+      <c r="J43" s="8">
         <v>609</v>
       </c>
-      <c r="N43" s="5">
+      <c r="K43" s="5">
         <v>224804.01700000008</v>
       </c>
-      <c r="O43" s="11">
+      <c r="L43" s="11">
         <v>2.6514153181171261E-2</v>
       </c>
-      <c r="P43" s="4">
+      <c r="M43" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="15" t="str">
         <f>+VLOOKUP(B44,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>MEGAMALL BUCARAMANGA</v>
@@ -8876,32 +8477,23 @@
       <c r="H44" s="8">
         <v>406</v>
       </c>
-      <c r="I44" s="4">
-        <v>0.17604</v>
-      </c>
-      <c r="J44" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K44" s="15">
-        <v>43</v>
-      </c>
-      <c r="L44" s="15" t="s">
+      <c r="I44" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M44" s="8">
+      <c r="J44" s="8">
         <v>545</v>
       </c>
-      <c r="N44" s="5">
+      <c r="K44" s="5">
         <v>238716.19799999997</v>
       </c>
-      <c r="O44" s="11">
+      <c r="L44" s="11">
         <v>2.5549774199882191E-2</v>
       </c>
-      <c r="P44" s="4">
+      <c r="M44" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="str">
         <f>+VLOOKUP(B45,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>SAN SILVESTRE BARRANCABERMEJA</v>
@@ -8927,32 +8519,23 @@
       <c r="H45" s="8">
         <v>412</v>
       </c>
-      <c r="I45" s="4">
-        <v>0.13397000000000001</v>
-      </c>
-      <c r="J45" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K45" s="15">
-        <v>44</v>
-      </c>
-      <c r="L45" s="15" t="s">
+      <c r="I45" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M45" s="8">
+      <c r="J45" s="8">
         <v>548</v>
       </c>
-      <c r="N45" s="5">
+      <c r="K45" s="5">
         <v>238416.40900000007</v>
       </c>
-      <c r="O45" s="11">
+      <c r="L45" s="11">
         <v>3.367890486282147E-2</v>
       </c>
-      <c r="P45" s="4">
+      <c r="M45" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="str">
         <f>+VLOOKUP(B46,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA OVIEDO 2</v>
@@ -8978,32 +8561,23 @@
       <c r="H46" s="8">
         <v>395</v>
       </c>
-      <c r="I46" s="4">
-        <v>0.109415</v>
-      </c>
-      <c r="J46" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K46" s="15">
-        <v>45</v>
-      </c>
-      <c r="L46" s="15" t="s">
+      <c r="I46" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M46" s="8">
+      <c r="J46" s="8">
         <v>564</v>
       </c>
-      <c r="N46" s="5">
+      <c r="K46" s="5">
         <v>277953.75300000014</v>
       </c>
-      <c r="O46" s="11">
+      <c r="L46" s="11">
         <v>3.951794915470766E-2</v>
       </c>
-      <c r="P46" s="4">
+      <c r="M46" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="str">
         <f>+VLOOKUP(B47,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA JARDINES DE LLANOGRANDE</v>
@@ -9029,32 +8603,23 @@
       <c r="H47" s="8">
         <v>443</v>
       </c>
-      <c r="I47" s="4">
-        <v>9.3427999999999997E-2</v>
-      </c>
-      <c r="J47" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K47" s="15">
-        <v>46</v>
-      </c>
-      <c r="L47" s="15" t="s">
+      <c r="I47" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M47" s="8">
+      <c r="J47" s="8">
         <v>604</v>
       </c>
-      <c r="N47" s="5">
+      <c r="K47" s="5">
         <v>274405.08700000012</v>
       </c>
-      <c r="O47" s="11">
+      <c r="L47" s="11">
         <v>5.4298642533936653E-2</v>
       </c>
-      <c r="P47" s="4">
+      <c r="M47" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="str">
         <f>+VLOOKUP(B48,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA ECOPLAZA BOGOTA</v>
@@ -9080,32 +8645,23 @@
       <c r="H48" s="8">
         <v>387</v>
       </c>
-      <c r="I48" s="4">
-        <v>7.7240000000000003E-2</v>
-      </c>
-      <c r="J48" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K48" s="15">
-        <v>47</v>
-      </c>
-      <c r="L48" s="15" t="s">
+      <c r="I48" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M48" s="8">
+      <c r="J48" s="8">
         <v>521</v>
       </c>
-      <c r="N48" s="5">
+      <c r="K48" s="5">
         <v>236612.11400000003</v>
       </c>
-      <c r="O48" s="11">
+      <c r="L48" s="11">
         <v>3.0744643389224478E-2</v>
       </c>
-      <c r="P48" s="4">
+      <c r="M48" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="str">
         <f>+VLOOKUP(B49,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA PRIMAVERA</v>
@@ -9131,32 +8687,23 @@
       <c r="H49" s="8">
         <v>442</v>
       </c>
-      <c r="I49" s="4">
-        <v>4.7275999999999999E-2</v>
-      </c>
-      <c r="J49" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K49" s="15">
-        <v>48</v>
-      </c>
-      <c r="L49" s="15" t="s">
+      <c r="I49" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M49" s="8">
+      <c r="J49" s="8">
         <v>592</v>
       </c>
-      <c r="N49" s="5">
+      <c r="K49" s="5">
         <v>237469.01700000008</v>
       </c>
-      <c r="O49" s="11">
+      <c r="L49" s="11">
         <v>2.8108623153882802E-2</v>
       </c>
-      <c r="P49" s="4">
+      <c r="M49" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="str">
         <f>+VLOOKUP(B50,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA UNICENTRO BOGOTÁ</v>
@@ -9182,32 +8729,23 @@
       <c r="H50" s="8">
         <v>334</v>
       </c>
-      <c r="I50" s="4">
-        <v>-7.1650000000000005E-2</v>
-      </c>
-      <c r="J50" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K50" s="15">
-        <v>49</v>
-      </c>
-      <c r="L50" s="15" t="s">
+      <c r="I50" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M50" s="8">
+      <c r="J50" s="8">
         <v>465</v>
       </c>
-      <c r="N50" s="5">
+      <c r="K50" s="5">
         <v>241176.42300000007</v>
       </c>
-      <c r="O50" s="11">
+      <c r="L50" s="11">
         <v>2.1233889710542995E-2</v>
       </c>
-      <c r="P50" s="4">
+      <c r="M50" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="15" t="str">
         <f>+VLOOKUP(B51,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>MAYALES VALLEDUPAR</v>
@@ -9233,32 +8771,23 @@
       <c r="H51" s="8">
         <v>389</v>
       </c>
-      <c r="I51" s="4">
-        <v>-7.8311000000000006E-2</v>
-      </c>
-      <c r="J51" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K51" s="15">
-        <v>50</v>
-      </c>
-      <c r="L51" s="15" t="s">
+      <c r="I51" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M51" s="8">
+      <c r="J51" s="8">
         <v>539</v>
       </c>
-      <c r="N51" s="5">
+      <c r="K51" s="5">
         <v>251574.68500000006</v>
       </c>
-      <c r="O51" s="11">
+      <c r="L51" s="11">
         <v>2.0778162558565898E-2</v>
       </c>
-      <c r="P51" s="4">
+      <c r="M51" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="15" t="str">
         <f>+VLOOKUP(B52,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA FONTANAR CHIA</v>
@@ -9284,32 +8813,23 @@
       <c r="H52" s="8">
         <v>333</v>
       </c>
-      <c r="I52" s="4">
-        <v>-9.3827999999999995E-2</v>
-      </c>
-      <c r="J52" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K52" s="15">
-        <v>51</v>
-      </c>
-      <c r="L52" s="15" t="s">
+      <c r="I52" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M52" s="8">
+      <c r="J52" s="8">
         <v>492</v>
       </c>
-      <c r="N52" s="5">
+      <c r="K52" s="5">
         <v>285672.64100000018</v>
       </c>
-      <c r="O52" s="11">
+      <c r="L52" s="11">
         <v>2.0759685876295998E-2</v>
       </c>
-      <c r="P52" s="4">
+      <c r="M52" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="str">
         <f>+VLOOKUP(B53,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA TINTAL</v>
@@ -9335,32 +8855,23 @@
       <c r="H53" s="8">
         <v>372</v>
       </c>
-      <c r="I53" s="4">
-        <v>-0.105604</v>
-      </c>
-      <c r="J53" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K53" s="15">
-        <v>52</v>
-      </c>
-      <c r="L53" s="15" t="s">
+      <c r="I53" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M53" s="8">
+      <c r="J53" s="8">
         <v>513</v>
       </c>
-      <c r="N53" s="5">
+      <c r="K53" s="5">
         <v>257460.51800000016</v>
       </c>
-      <c r="O53" s="11">
+      <c r="L53" s="11">
         <v>3.4733919060408798E-2</v>
       </c>
-      <c r="P53" s="4">
+      <c r="M53" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="15" t="str">
         <f>+VLOOKUP(B54,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA PLAZA DE LAS AMERICAS</v>
@@ -9386,32 +8897,23 @@
       <c r="H54" s="8">
         <v>361</v>
       </c>
-      <c r="I54" s="4">
-        <v>-0.10589999999999999</v>
-      </c>
-      <c r="J54" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K54" s="15">
-        <v>53</v>
-      </c>
-      <c r="L54" s="15" t="s">
+      <c r="I54" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M54" s="8">
+      <c r="J54" s="8">
         <v>508</v>
       </c>
-      <c r="N54" s="5">
+      <c r="K54" s="5">
         <v>252784.42900000006</v>
       </c>
-      <c r="O54" s="11">
+      <c r="L54" s="11">
         <v>2.5287290931846628E-2</v>
       </c>
-      <c r="P54" s="4">
+      <c r="M54" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="str">
         <f>+VLOOKUP(B55,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA NUESTRA URABA</v>
@@ -9437,32 +8939,23 @@
       <c r="H55" s="8">
         <v>381</v>
       </c>
-      <c r="I55" s="4">
-        <v>-0.152395</v>
-      </c>
-      <c r="J55" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K55" s="15">
-        <v>54</v>
-      </c>
-      <c r="L55" s="15" t="s">
+      <c r="I55" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M55" s="8">
+      <c r="J55" s="8">
         <v>503</v>
       </c>
-      <c r="N55" s="5">
+      <c r="K55" s="5">
         <v>261074.06000000006</v>
       </c>
-      <c r="O55" s="11">
+      <c r="L55" s="11">
         <v>2.1976931663152673E-2</v>
       </c>
-      <c r="P55" s="4">
+      <c r="M55" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="15" t="str">
         <f>+VLOOKUP(B56,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>BUENAVISTA SANTA MARTA</v>
@@ -9488,32 +8981,23 @@
       <c r="H56" s="8">
         <v>332</v>
       </c>
-      <c r="I56" s="4">
-        <v>-0.171542</v>
-      </c>
-      <c r="J56" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K56" s="15">
-        <v>55</v>
-      </c>
-      <c r="L56" s="15" t="s">
+      <c r="I56" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M56" s="8">
+      <c r="J56" s="8">
         <v>452</v>
       </c>
-      <c r="N56" s="5">
+      <c r="K56" s="5">
         <v>267773.78000000009</v>
       </c>
-      <c r="O56" s="11">
+      <c r="L56" s="11">
         <v>2.2876537223960859E-2</v>
       </c>
-      <c r="P56" s="4">
+      <c r="M56" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="15" t="str">
         <f>+VLOOKUP(B57,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>LA CASTELLANA CARTAGENA</v>
@@ -9539,32 +9023,23 @@
       <c r="H57" s="8">
         <v>355</v>
       </c>
-      <c r="I57" s="4">
-        <v>-0.272588</v>
-      </c>
-      <c r="J57" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K57" s="15">
-        <v>56</v>
-      </c>
-      <c r="L57" s="15" t="s">
+      <c r="I57" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M57" s="8">
+      <c r="J57" s="8">
         <v>496</v>
       </c>
-      <c r="N57" s="5">
+      <c r="K57" s="5">
         <v>259130.10400000008</v>
       </c>
-      <c r="O57" s="11">
+      <c r="L57" s="11">
         <v>2.0159916634937176E-2</v>
       </c>
-      <c r="P57" s="4">
+      <c r="M57" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="15" t="str">
         <f>+VLOOKUP(B58,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA GRAN PLAZA IPIALES</v>
@@ -9590,32 +9065,23 @@
       <c r="H58" s="8">
         <v>348</v>
       </c>
-      <c r="I58" s="4">
-        <v>-0.28082400000000002</v>
-      </c>
-      <c r="J58" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K58" s="15">
-        <v>57</v>
-      </c>
-      <c r="L58" s="15" t="s">
+      <c r="I58" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M58" s="8">
+      <c r="J58" s="8">
         <v>493</v>
       </c>
-      <c r="N58" s="5">
+      <c r="K58" s="5">
         <v>271532.28100000008</v>
       </c>
-      <c r="O58" s="11">
+      <c r="L58" s="11">
         <v>2.480959779923075E-2</v>
       </c>
-      <c r="P58" s="4">
+      <c r="M58" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="15" t="str">
         <f>+VLOOKUP(B59,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>UNICENTRO CUCUTA</v>
@@ -9641,32 +9107,23 @@
       <c r="H59" s="8">
         <v>348</v>
       </c>
-      <c r="I59" s="4">
-        <v>-0.307612</v>
-      </c>
-      <c r="J59" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K59" s="15">
-        <v>58</v>
-      </c>
-      <c r="L59" s="15" t="s">
+      <c r="I59" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M59" s="8">
+      <c r="J59" s="8">
         <v>494</v>
       </c>
-      <c r="N59" s="5">
+      <c r="K59" s="5">
         <v>226004.86500000002</v>
       </c>
-      <c r="O59" s="11">
+      <c r="L59" s="11">
         <v>2.0465520324995528E-2</v>
       </c>
-      <c r="P59" s="4">
+      <c r="M59" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="str">
         <f>+VLOOKUP(B60,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA DIVERPLAZA BOGOTÁ</v>
@@ -9692,32 +9149,23 @@
       <c r="H60" s="8">
         <v>280</v>
       </c>
-      <c r="I60" s="4">
-        <v>-0.32542199999999999</v>
-      </c>
-      <c r="J60" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K60" s="15">
-        <v>59</v>
-      </c>
-      <c r="L60" s="15" t="s">
+      <c r="I60" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M60" s="8">
+      <c r="J60" s="8">
         <v>411</v>
       </c>
-      <c r="N60" s="5">
+      <c r="K60" s="5">
         <v>297008.75800000009</v>
       </c>
-      <c r="O60" s="11">
+      <c r="L60" s="11">
         <v>2.8118180292093335E-2</v>
       </c>
-      <c r="P60" s="4">
+      <c r="M60" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="str">
         <f>+VLOOKUP(B61,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA SANTAFÉ BOGOTÁ</v>
@@ -9743,32 +9191,23 @@
       <c r="H61" s="8">
         <v>313</v>
       </c>
-      <c r="I61" s="4">
-        <v>-0.34187499999999998</v>
-      </c>
-      <c r="J61" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K61" s="15">
-        <v>60</v>
-      </c>
-      <c r="L61" s="15" t="s">
+      <c r="I61" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M61" s="8">
+      <c r="J61" s="8">
         <v>462</v>
       </c>
-      <c r="N61" s="5">
+      <c r="K61" s="5">
         <v>250055.88000000003</v>
       </c>
-      <c r="O61" s="11">
+      <c r="L61" s="11">
         <v>2.4509803921568627E-2</v>
       </c>
-      <c r="P61" s="4">
+      <c r="M61" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="15" t="str">
         <f>+VLOOKUP(B62,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>CAMPANARIO POPAYAN</v>
@@ -9794,32 +9233,23 @@
       <c r="H62" s="8">
         <v>302</v>
       </c>
-      <c r="I62" s="4">
-        <v>-0.38361299999999998</v>
-      </c>
-      <c r="J62" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K62" s="15">
-        <v>61</v>
-      </c>
-      <c r="L62" s="15" t="s">
+      <c r="I62" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M62" s="8">
+      <c r="J62" s="8">
         <v>435</v>
       </c>
-      <c r="N62" s="5">
+      <c r="K62" s="5">
         <v>251593.58900000004</v>
       </c>
-      <c r="O62" s="11">
+      <c r="L62" s="11">
         <v>1.473460576362951E-2</v>
       </c>
-      <c r="P62" s="4">
+      <c r="M62" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="15" t="str">
         <f>+VLOOKUP(B63,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA PORTAL 80</v>
@@ -9845,32 +9275,23 @@
       <c r="H63" s="8">
         <v>278</v>
       </c>
-      <c r="I63" s="4">
-        <v>-0.45447300000000002</v>
-      </c>
-      <c r="J63" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K63" s="15">
-        <v>62</v>
-      </c>
-      <c r="L63" s="15" t="s">
+      <c r="I63" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M63" s="8">
+      <c r="J63" s="8">
         <v>418</v>
       </c>
-      <c r="N63" s="5">
+      <c r="K63" s="5">
         <v>271564.58199999999</v>
       </c>
-      <c r="O63" s="11">
+      <c r="L63" s="11">
         <v>3.0779054916985953E-2</v>
       </c>
-      <c r="P63" s="4">
+      <c r="M63" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="15" t="str">
         <f>+VLOOKUP(B64,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>CACIQUE BUCARAMANGA</v>
@@ -9896,32 +9317,23 @@
       <c r="H64" s="8">
         <v>308</v>
       </c>
-      <c r="I64" s="4">
-        <v>-0.56712399999999996</v>
-      </c>
-      <c r="J64" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K64" s="15">
-        <v>63</v>
-      </c>
-      <c r="L64" s="15" t="s">
+      <c r="I64" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M64" s="8">
+      <c r="J64" s="8">
         <v>437</v>
       </c>
-      <c r="N64" s="5">
+      <c r="K64" s="5">
         <v>208537.64100000009</v>
       </c>
-      <c r="O64" s="11">
+      <c r="L64" s="11">
         <v>1.6699630234757932E-2</v>
       </c>
-      <c r="P64" s="4">
+      <c r="M64" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="15" t="str">
         <f>+VLOOKUP(B65,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>BUENAVISTA BARRANQUILLA</v>
@@ -9947,32 +9359,23 @@
       <c r="H65" s="8">
         <v>319</v>
       </c>
-      <c r="I65" s="4">
-        <v>-0.58732200000000001</v>
-      </c>
-      <c r="J65" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K65" s="15">
-        <v>64</v>
-      </c>
-      <c r="L65" s="15" t="s">
+      <c r="I65" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M65" s="8">
+      <c r="J65" s="8">
         <v>452</v>
       </c>
-      <c r="N65" s="5">
+      <c r="K65" s="5">
         <v>212023.94700000001</v>
       </c>
-      <c r="O65" s="11">
+      <c r="L65" s="11">
         <v>1.6249005568814638E-2</v>
       </c>
-      <c r="P65" s="4">
+      <c r="M65" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="15" t="str">
         <f>+VLOOKUP(B66,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA PLAZA CLARO</v>
@@ -9998,32 +9401,23 @@
       <c r="H66" s="8">
         <v>272</v>
       </c>
-      <c r="I66" s="4">
-        <v>-0.60035899999999998</v>
-      </c>
-      <c r="J66" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K66" s="15">
-        <v>65</v>
-      </c>
-      <c r="L66" s="15" t="s">
+      <c r="I66" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M66" s="8">
+      <c r="J66" s="8">
         <v>418</v>
       </c>
-      <c r="N66" s="5">
+      <c r="K66" s="5">
         <v>257470.22100000014</v>
       </c>
-      <c r="O66" s="11">
+      <c r="L66" s="11">
         <v>3.291915442956269E-2</v>
       </c>
-      <c r="P66" s="4">
+      <c r="M66" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="str">
         <f>+VLOOKUP(B67,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA CALIMA</v>
@@ -10049,32 +9443,23 @@
       <c r="H67" s="8">
         <v>277</v>
       </c>
-      <c r="I67" s="4">
-        <v>-0.64625600000000005</v>
-      </c>
-      <c r="J67" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K67" s="15">
-        <v>66</v>
-      </c>
-      <c r="L67" s="15" t="s">
+      <c r="I67" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M67" s="8">
+      <c r="J67" s="8">
         <v>419</v>
       </c>
-      <c r="N67" s="5">
+      <c r="K67" s="5">
         <v>238401.02100000015</v>
       </c>
-      <c r="O67" s="11">
+      <c r="L67" s="11">
         <v>2.2485207100591716E-2</v>
       </c>
-      <c r="P67" s="4">
+      <c r="M67" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="str">
         <f>+VLOOKUP(B68,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA HAYUELOS</v>
@@ -10100,32 +9485,23 @@
       <c r="H68" s="8">
         <v>261</v>
       </c>
-      <c r="I68" s="4">
-        <v>-0.74871600000000005</v>
-      </c>
-      <c r="J68" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K68" s="15">
-        <v>67</v>
-      </c>
-      <c r="L68" s="15" t="s">
+      <c r="I68" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M68" s="8">
+      <c r="J68" s="8">
         <v>396</v>
       </c>
-      <c r="N68" s="5">
+      <c r="K68" s="5">
         <v>247922.859</v>
       </c>
-      <c r="O68" s="11">
+      <c r="L68" s="11">
         <v>3.0897091175751651E-2</v>
       </c>
-      <c r="P68" s="4">
+      <c r="M68" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="str">
         <f>+VLOOKUP(B69,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA  SAN ANDRES  2</v>
@@ -10151,32 +9527,23 @@
       <c r="H69" s="8">
         <v>303</v>
       </c>
-      <c r="I69" s="4">
-        <v>-0.88341899999999995</v>
-      </c>
-      <c r="J69" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K69" s="15">
-        <v>68</v>
-      </c>
-      <c r="L69" s="15" t="s">
+      <c r="I69" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M69" s="8">
+      <c r="J69" s="8">
         <v>373</v>
       </c>
-      <c r="N69" s="5">
+      <c r="K69" s="5">
         <v>142721.804</v>
       </c>
-      <c r="O69" s="11">
+      <c r="L69" s="11">
         <v>9.4257959026642305E-3</v>
       </c>
-      <c r="P69" s="4">
+      <c r="M69" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="15" t="str">
         <f>+VLOOKUP(B70,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA PASEO VILLA DEL RIO</v>
@@ -10202,32 +9569,23 @@
       <c r="H70" s="8">
         <v>236</v>
       </c>
-      <c r="I70" s="4">
-        <v>-0.96509299999999998</v>
-      </c>
-      <c r="J70" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="K70" s="15">
-        <v>69</v>
-      </c>
-      <c r="L70" s="15" t="s">
+      <c r="I70" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M70" s="8">
+      <c r="J70" s="8">
         <v>373</v>
       </c>
-      <c r="N70" s="5">
+      <c r="K70" s="5">
         <v>216114.08899999998</v>
       </c>
-      <c r="O70" s="11">
+      <c r="L70" s="11">
         <v>2.9256442754541614E-2</v>
       </c>
-      <c r="P70" s="4">
+      <c r="M70" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="15" t="str">
         <f>+VLOOKUP(B71,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>MULTICENTRO IBAGUE</v>
@@ -10253,32 +9611,23 @@
       <c r="H71" s="8">
         <v>220</v>
       </c>
-      <c r="I71" s="4">
-        <v>-1.2904709999999999</v>
-      </c>
-      <c r="J71" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K71" s="15">
-        <v>70</v>
-      </c>
-      <c r="L71" s="15" t="s">
+      <c r="I71" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M71" s="8">
+      <c r="J71" s="8">
         <v>358</v>
       </c>
-      <c r="N71" s="5">
+      <c r="K71" s="5">
         <v>214603.04100000008</v>
       </c>
-      <c r="O71" s="11">
+      <c r="L71" s="11">
         <v>2.1051081996172529E-2</v>
       </c>
-      <c r="P71" s="4">
+      <c r="M71" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="15" t="str">
         <f>+VLOOKUP(B72,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>OFFCORSS VIVA  TUNJA</v>
@@ -10304,32 +9653,23 @@
       <c r="H72" s="8">
         <v>192</v>
       </c>
-      <c r="I72" s="4">
-        <v>-1.3027500000000001</v>
-      </c>
-      <c r="J72" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K72" s="15">
-        <v>71</v>
-      </c>
-      <c r="L72" s="15" t="s">
+      <c r="I72" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M72" s="8">
+      <c r="J72" s="8">
         <v>333</v>
       </c>
-      <c r="N72" s="5">
+      <c r="K72" s="5">
         <v>202515.72500000003</v>
       </c>
-      <c r="O72" s="11">
+      <c r="L72" s="11">
         <v>1.7003223048082616E-2</v>
       </c>
-      <c r="P72" s="4">
+      <c r="M72" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="15" t="str">
         <f>+VLOOKUP(B73,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>OFFCORSS ALCARAVAN</v>
@@ -10355,32 +9695,23 @@
       <c r="H73" s="8">
         <v>207</v>
       </c>
-      <c r="I73" s="4">
-        <v>-1.316978</v>
-      </c>
-      <c r="J73" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K73" s="15">
-        <v>72</v>
-      </c>
-      <c r="L73" s="15" t="s">
+      <c r="I73" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M73" s="8">
+      <c r="J73" s="8">
         <v>297</v>
       </c>
-      <c r="N73" s="5">
+      <c r="K73" s="5">
         <v>262809.01199999999</v>
       </c>
-      <c r="O73" s="11">
+      <c r="L73" s="11">
         <v>1.9656659815302666E-2</v>
       </c>
-      <c r="P73" s="4">
+      <c r="M73" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="15" t="str">
         <f>+VLOOKUP(B74,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>PORTAL DE PRADO BARRANQUILLA</v>
@@ -10406,32 +9737,23 @@
       <c r="H74" s="8">
         <v>182</v>
       </c>
-      <c r="I74" s="4">
-        <v>-1.46065</v>
-      </c>
-      <c r="J74" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K74" s="15">
-        <v>73</v>
-      </c>
-      <c r="L74" s="15" t="s">
+      <c r="I74" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M74" s="8">
+      <c r="J74" s="8">
         <v>337</v>
       </c>
-      <c r="N74" s="5">
+      <c r="K74" s="5">
         <v>260294.01600000006</v>
       </c>
-      <c r="O74" s="11">
+      <c r="L74" s="11">
         <v>2.5016491601968845E-2</v>
       </c>
-      <c r="P74" s="4">
+      <c r="M74" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="15" t="str">
         <f>+VLOOKUP(B75,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>OFFCORSS PASTO</v>
@@ -10457,32 +9779,23 @@
       <c r="H75" s="8">
         <v>205</v>
       </c>
-      <c r="I75" s="4">
-        <v>-1.5145420000000001</v>
-      </c>
-      <c r="J75" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K75" s="15">
-        <v>74</v>
-      </c>
-      <c r="L75" s="15" t="s">
+      <c r="I75" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M75" s="8">
+      <c r="J75" s="8">
         <v>338</v>
       </c>
-      <c r="N75" s="5">
+      <c r="K75" s="5">
         <v>224233.61600000004</v>
       </c>
-      <c r="O75" s="11">
+      <c r="L75" s="11">
         <v>1.5353612897034833E-2</v>
       </c>
-      <c r="P75" s="4">
+      <c r="M75" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="str">
         <f>+VLOOKUP(B76,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>DUITAMA BOYACA</v>
@@ -10508,32 +9821,23 @@
       <c r="H76" s="8">
         <v>168</v>
       </c>
-      <c r="I76" s="4">
-        <v>-1.867651</v>
-      </c>
-      <c r="J76" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K76" s="15">
-        <v>75</v>
-      </c>
-      <c r="L76" s="15" t="s">
+      <c r="I76" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M76" s="8">
+      <c r="J76" s="8">
         <v>295</v>
       </c>
-      <c r="N76" s="5">
+      <c r="K76" s="5">
         <v>165315.56700000001</v>
       </c>
-      <c r="O76" s="11">
+      <c r="L76" s="11">
         <v>1.9620980091883615E-2</v>
       </c>
-      <c r="P76" s="4">
+      <c r="M76" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="str">
         <f>+VLOOKUP(B77,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>OFFCORSS SOGAMOSO</v>
@@ -10559,32 +9863,23 @@
       <c r="H77" s="8">
         <v>147</v>
       </c>
-      <c r="I77" s="4">
-        <v>-2.0231210000000002</v>
-      </c>
-      <c r="J77" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K77" s="15">
-        <v>76</v>
-      </c>
-      <c r="L77" s="15" t="s">
+      <c r="I77" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M77" s="8">
+      <c r="J77" s="8">
         <v>275</v>
       </c>
-      <c r="N77" s="5">
+      <c r="K77" s="5">
         <v>146542.56900000002</v>
       </c>
-      <c r="O77" s="11">
+      <c r="L77" s="11">
         <v>2.3128227194492253E-2</v>
       </c>
-      <c r="P77" s="4">
+      <c r="M77" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="15" t="str">
         <f>+VLOOKUP(B78,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>OCAÑA</v>
@@ -10610,32 +9905,23 @@
       <c r="H78" s="8">
         <v>141</v>
       </c>
-      <c r="I78" s="4">
-        <v>-2.030942</v>
-      </c>
-      <c r="J78" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K78" s="15">
-        <v>77</v>
-      </c>
-      <c r="L78" s="15" t="s">
+      <c r="I78" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M78" s="8">
+      <c r="J78" s="8">
         <v>247</v>
       </c>
-      <c r="N78" s="5">
+      <c r="K78" s="5">
         <v>211037.04800000004</v>
       </c>
-      <c r="O78" s="11">
+      <c r="L78" s="11">
         <v>7.6749677973379131E-3</v>
       </c>
-      <c r="P78" s="4">
+      <c r="M78" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="15" t="str">
         <f>+VLOOKUP(B79,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA PARQUE ALEGRA</v>
@@ -10661,32 +9947,23 @@
       <c r="H79" s="8">
         <v>133</v>
       </c>
-      <c r="I79" s="4">
-        <v>-2.058557</v>
-      </c>
-      <c r="J79" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K79" s="15">
-        <v>78</v>
-      </c>
-      <c r="L79" s="15" t="s">
+      <c r="I79" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M79" s="8">
+      <c r="J79" s="8">
         <v>281</v>
       </c>
-      <c r="N79" s="5">
+      <c r="K79" s="5">
         <v>160223.42199999999</v>
       </c>
-      <c r="O79" s="11">
+      <c r="L79" s="11">
         <v>1.248464190876303E-2</v>
       </c>
-      <c r="P79" s="4">
+      <c r="M79" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="15" t="str">
         <f>+VLOOKUP(B80,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>VICTORIA PEREIRA</v>
@@ -10712,32 +9989,23 @@
       <c r="H80" s="8">
         <v>159</v>
       </c>
-      <c r="I80" s="4">
-        <v>-2.2747570000000001</v>
-      </c>
-      <c r="J80" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K80" s="15">
-        <v>79</v>
-      </c>
-      <c r="L80" s="15" t="s">
+      <c r="I80" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M80" s="8">
+      <c r="J80" s="8">
         <v>232</v>
       </c>
-      <c r="N80" s="5">
+      <c r="K80" s="5">
         <v>73406.840000000011</v>
       </c>
-      <c r="O80" s="11">
+      <c r="L80" s="11">
         <v>1.2822156686754712E-2</v>
       </c>
-      <c r="P80" s="4">
+      <c r="M80" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="15" t="str">
         <f>+VLOOKUP(B81,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>OFFCORSS FACATATIVA</v>
@@ -10763,32 +10031,23 @@
       <c r="H81" s="8">
         <v>141</v>
       </c>
-      <c r="I81" s="4">
-        <v>-2.5495269999999999</v>
-      </c>
-      <c r="J81" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K81" s="15">
-        <v>80</v>
-      </c>
-      <c r="L81" s="15" t="s">
+      <c r="I81" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M81" s="8">
+      <c r="J81" s="8">
         <v>259</v>
       </c>
-      <c r="N81" s="5">
+      <c r="K81" s="5">
         <v>133247.01199999999</v>
       </c>
-      <c r="O81" s="11">
+      <c r="L81" s="11">
         <v>2.2723759468233112E-2</v>
       </c>
-      <c r="P81" s="4">
+      <c r="M81" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="15" t="str">
         <f>+VLOOKUP(B82,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>OFFCORSS AGUACHICA</v>
@@ -10814,32 +10073,23 @@
       <c r="H82" s="8">
         <v>117</v>
       </c>
-      <c r="I82" s="4">
-        <v>-2.6019779999999999</v>
-      </c>
-      <c r="J82" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K82" s="15">
-        <v>81</v>
-      </c>
-      <c r="L82" s="15" t="s">
+      <c r="I82" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M82" s="8">
+      <c r="J82" s="8">
         <v>250</v>
       </c>
-      <c r="N82" s="5">
+      <c r="K82" s="5">
         <v>187804.84499999997</v>
       </c>
-      <c r="O82" s="11">
+      <c r="L82" s="11">
         <v>2.587142684838982E-2</v>
       </c>
-      <c r="P82" s="4">
+      <c r="M82" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="15" t="str">
         <f>+VLOOKUP(B83,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA OFFCORSS TULUA</v>
@@ -10865,32 +10115,23 @@
       <c r="H83" s="8">
         <v>127</v>
       </c>
-      <c r="I83" s="4">
-        <v>-3.3456220000000001</v>
-      </c>
-      <c r="J83" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K83" s="15">
-        <v>82</v>
-      </c>
-      <c r="L83" s="15" t="s">
+      <c r="I83" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M83" s="8">
+      <c r="J83" s="8">
         <v>226</v>
       </c>
-      <c r="N83" s="5">
+      <c r="K83" s="5">
         <v>80551.622000000003</v>
       </c>
-      <c r="O83" s="11">
+      <c r="L83" s="11">
         <v>3.8723181580324437E-2</v>
       </c>
-      <c r="P83" s="4">
+      <c r="M83" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="15" t="str">
         <f>+VLOOKUP(B84,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>OFFCORSS GRANADA</v>
@@ -10916,32 +10157,23 @@
       <c r="H84" s="8">
         <v>75</v>
       </c>
-      <c r="I84" s="4">
-        <v>-3.5233189999999999</v>
-      </c>
-      <c r="J84" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K84" s="15">
-        <v>83</v>
-      </c>
-      <c r="L84" s="15" t="s">
+      <c r="I84" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M84" s="8">
+      <c r="J84" s="8">
         <v>186</v>
       </c>
-      <c r="N84" s="5">
+      <c r="K84" s="5">
         <v>129393.71199999998</v>
       </c>
-      <c r="O84" s="11">
+      <c r="L84" s="11">
         <v>1.1670936521491603E-2</v>
       </c>
-      <c r="P84" s="4">
+      <c r="M84" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="15" t="str">
         <f>+VLOOKUP(B85,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>OFFCORSS VILLANUEVA</v>
@@ -10967,32 +10199,23 @@
       <c r="H85" s="8">
         <v>30</v>
       </c>
-      <c r="I85" s="4">
-        <v>-4.7424039999999996</v>
-      </c>
-      <c r="J85" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K85" s="15">
-        <v>84</v>
-      </c>
-      <c r="L85" s="15" t="s">
+      <c r="I85" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M85" s="8">
+      <c r="J85" s="8">
         <v>110</v>
       </c>
-      <c r="N85" s="5">
+      <c r="K85" s="5">
         <v>47019.164000000004</v>
       </c>
-      <c r="O85" s="11">
+      <c r="L85" s="11">
         <v>3.1023784901758014E-2</v>
       </c>
-      <c r="P85" s="4">
+      <c r="M85" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="15" t="str">
         <f>+VLOOKUP(B86,'[1]Tiendas Cuidado personal'!$B:$C,2,0)</f>
         <v>TIENDA  ARRAYANES</v>
@@ -11018,28 +10241,19 @@
       <c r="H86" s="8">
         <v>2</v>
       </c>
-      <c r="I86" s="4">
-        <v>-6.2766460000000004</v>
-      </c>
-      <c r="J86" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K86" s="15">
-        <v>85</v>
-      </c>
-      <c r="L86" s="15" t="s">
+      <c r="I86" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="M86" s="8">
-        <v>0</v>
-      </c>
-      <c r="N86" s="5">
+      <c r="J86" s="8">
+        <v>0</v>
+      </c>
+      <c r="K86" s="5">
         <v>5.9309999999999992</v>
       </c>
-      <c r="O86" s="11">
+      <c r="L86" s="11">
         <v>4.2105263157894736E-3</v>
       </c>
-      <c r="P86" s="4">
+      <c r="M86" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>